<commit_message>
POI practiced on excel file write,style and read
</commit_message>
<xml_diff>
--- a/Apache-POI/users.xlsx
+++ b/Apache-POI/users.xlsx
@@ -17,7 +17,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>age</t>
+    <t>Age</t>
   </si>
   <si>
     <t>haridas</t>
@@ -46,13 +46,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -63,7 +68,7 @@
       <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -71,12 +76,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -88,12 +114,16 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="7.82421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="4.0703125" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>